<commit_message>
Se agrego el CSS de Multinacional de Seguros
</commit_message>
<xml_diff>
--- a/convenios/multinacional.xlsx
+++ b/convenios/multinacional.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16560" tabRatio="448" activeTab="3"/>
+    <workbookView xWindow="2240" yWindow="2220" windowWidth="23360" windowHeight="12340" tabRatio="448" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_tasa_casco" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="tbl_re_tipo_cob_as" sheetId="3" r:id="rId3"/>
     <sheet name="tbl_grua" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -328,8 +328,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,25 +456,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+  <cellStyles count="31">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -794,20 +818,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="3"/>
-    <col min="2" max="2" width="14.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.625" style="3"/>
+    <col min="6" max="6" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7">
@@ -2312,6 +2336,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2324,16 +2349,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2930,23 +2955,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:J90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="12"/>
-    <col min="2" max="2" width="9.75" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="12"/>
+    <col min="2" max="2" width="9.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.375" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="3"/>
+    <col min="10" max="10" width="6.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" s="3" customFormat="1">
@@ -5208,10 +5233,10 @@
   <dimension ref="B3:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4:E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="3" spans="2:5">
       <c r="B3" s="36" t="s">
@@ -6153,6 +6178,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>